<commit_message>
Fix waste inputs in inventories + Version bump
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-BIGCC.xlsx
+++ b/premise/data/additional_inventories/lci-BIGCC.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sacchi_r\Documents\GitHub\premise\premise\data\additional_inventories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DDC2A7-4373-3E49-BEB7-096D6C3B8FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="10" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -230,7 +241,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -565,20 +576,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71.5546875" customWidth="1"/>
+    <col min="1" max="1" width="71.5" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -586,7 +597,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -594,7 +605,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -602,7 +613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -610,7 +621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -618,7 +629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -626,7 +637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -634,7 +645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -642,7 +653,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -650,12 +661,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -696,7 +707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -725,7 +736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -764,7 +775,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -803,7 +814,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -841,7 +852,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -861,7 +872,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -881,7 +892,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -902,7 +913,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -923,7 +934,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -941,7 +952,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -959,7 +970,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -977,7 +988,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -995,7 +1006,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -1013,7 +1024,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1031,7 +1042,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1049,7 +1060,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1067,7 +1078,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1088,7 +1099,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>1</v>
       </c>
@@ -1096,7 +1107,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -1104,7 +1115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1112,7 +1123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1120,7 +1131,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1128,7 +1139,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -1136,7 +1147,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1144,7 +1155,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -1152,12 +1163,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -1198,7 +1209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -1227,7 +1238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>24</v>
       </c>
@@ -1266,7 +1277,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>28</v>
       </c>
@@ -1305,7 +1316,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -1343,7 +1354,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>38</v>
       </c>
@@ -1363,7 +1374,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>35</v>
       </c>
@@ -1383,7 +1394,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -1404,7 +1415,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -1425,7 +1436,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>46</v>
       </c>
@@ -1443,7 +1454,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -1461,7 +1472,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -1479,7 +1490,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -1497,7 +1508,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>51</v>
       </c>
@@ -1515,7 +1526,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -1533,7 +1544,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>53</v>
       </c>
@@ -1551,7 +1562,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -1569,7 +1580,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -1590,7 +1601,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -1611,7 +1622,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>1</v>
       </c>
@@ -1619,7 +1630,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>2</v>
       </c>
@@ -1627,7 +1638,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -1635,7 +1646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -1643,7 +1654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -1651,7 +1662,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>9</v>
       </c>
@@ -1659,7 +1670,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>33</v>
       </c>
@@ -1667,7 +1678,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -1675,12 +1686,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -1721,7 +1732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>60</v>
       </c>
@@ -1750,7 +1761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>24</v>
       </c>
@@ -1789,7 +1800,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -1828,7 +1839,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>31</v>
       </c>
@@ -1866,7 +1877,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>38</v>
       </c>
@@ -1886,7 +1897,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>35</v>
       </c>
@@ -1906,7 +1917,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>42</v>
       </c>
@@ -1927,7 +1938,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>55</v>
       </c>
@@ -1948,7 +1959,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>46</v>
       </c>
@@ -1966,7 +1977,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -1984,7 +1995,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>49</v>
       </c>
@@ -2002,7 +2013,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>50</v>
       </c>
@@ -2020,7 +2031,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>51</v>
       </c>
@@ -2038,7 +2049,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>52</v>
       </c>
@@ -2056,7 +2067,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>53</v>
       </c>
@@ -2074,7 +2085,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>54</v>
       </c>
@@ -2092,7 +2103,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>56</v>
       </c>
@@ -2113,7 +2124,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Implements high voltage markets
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-BIGCC.xlsx
+++ b/premise/data/additional_inventories/lci-BIGCC.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DDC2A7-4373-3E49-BEB7-096D6C3B8FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EB23A4-4C9A-1541-9912-ABEDDD7FD8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateCount="10" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -741,8 +741,8 @@
         <v>24</v>
       </c>
       <c r="B14" s="4">
-        <f>1/(12500*8760*25)</f>
-        <v>3.6529680365296802E-10</v>
+        <f>1/(450000*8760*25)</f>
+        <v>1.0147133434804668E-11</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -780,8 +780,8 @@
         <v>28</v>
       </c>
       <c r="B15" s="4">
-        <f>1/(12500*8760*25)</f>
-        <v>3.6529680365296802E-10</v>
+        <f>1/(450000*8760*25)</f>
+        <v>1.0147133434804668E-11</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1243,8 +1243,8 @@
         <v>24</v>
       </c>
       <c r="B44" s="4">
-        <f>1/(12500*8760*25)</f>
-        <v>3.6529680365296802E-10</v>
+        <f>1/(450000*8760*25)</f>
+        <v>1.0147133434804668E-11</v>
       </c>
       <c r="C44" t="s">
         <v>3</v>
@@ -1282,8 +1282,8 @@
         <v>28</v>
       </c>
       <c r="B45" s="4">
-        <f>1/(12500*8760*25)</f>
-        <v>3.6529680365296802E-10</v>
+        <f>1/(450000*8760*25)</f>
+        <v>1.0147133434804668E-11</v>
       </c>
       <c r="C45" t="s">
         <v>3</v>
@@ -1766,8 +1766,8 @@
         <v>24</v>
       </c>
       <c r="B75" s="4">
-        <f>1/(12500*8760*25)</f>
-        <v>3.6529680365296802E-10</v>
+        <f>1/(450000*8760*25)</f>
+        <v>1.0147133434804668E-11</v>
       </c>
       <c r="C75" t="s">
         <v>3</v>
@@ -1805,8 +1805,8 @@
         <v>28</v>
       </c>
       <c r="B76" s="4">
-        <f>1/(12500*8760*25)</f>
-        <v>3.6529680365296802E-10</v>
+        <f>1/(450000*8760*25)</f>
+        <v>1.0147133434804668E-11</v>
       </c>
       <c r="C76" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Fix BIGCC inventories: plant requirement was too high.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-BIGCC.xlsx
+++ b/premise/data/additional_inventories/lci-BIGCC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DDC2A7-4373-3E49-BEB7-096D6C3B8FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400E60F4-8CFB-1341-AF28-F7A65899BFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -741,8 +741,8 @@
         <v>24</v>
       </c>
       <c r="B14" s="4">
-        <f>1/(12500*8760*25)</f>
-        <v>3.6529680365296802E-10</v>
+        <f>1/(450000*8760*25)</f>
+        <v>1.0147133434804668E-11</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -780,8 +780,8 @@
         <v>28</v>
       </c>
       <c r="B15" s="4">
-        <f>1/(12500*8760*25)</f>
-        <v>3.6529680365296802E-10</v>
+        <f>1/(450000*8760*25)</f>
+        <v>1.0147133434804668E-11</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1243,8 +1243,8 @@
         <v>24</v>
       </c>
       <c r="B44" s="4">
-        <f>1/(12500*8760*25)</f>
-        <v>3.6529680365296802E-10</v>
+        <f>1/(450000*8760*25)</f>
+        <v>1.0147133434804668E-11</v>
       </c>
       <c r="C44" t="s">
         <v>3</v>
@@ -1282,8 +1282,8 @@
         <v>28</v>
       </c>
       <c r="B45" s="4">
-        <f>1/(12500*8760*25)</f>
-        <v>3.6529680365296802E-10</v>
+        <f>1/(450000*8760*25)</f>
+        <v>1.0147133434804668E-11</v>
       </c>
       <c r="C45" t="s">
         <v>3</v>
@@ -1766,8 +1766,8 @@
         <v>24</v>
       </c>
       <c r="B75" s="4">
-        <f>1/(12500*8760*25)</f>
-        <v>3.6529680365296802E-10</v>
+        <f>1/(450000*8760*25)</f>
+        <v>1.0147133434804668E-11</v>
       </c>
       <c r="C75" t="s">
         <v>3</v>
@@ -1805,8 +1805,8 @@
         <v>28</v>
       </c>
       <c r="B76" s="4">
-        <f>1/(12500*8760*25)</f>
-        <v>3.6529680365296802E-10</v>
+        <f>1/(450000*8760*25)</f>
+        <v>1.0147133434804668E-11</v>
       </c>
       <c r="C76" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Fix the carbon balance for the biomass markets
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-BIGCC.xlsx
+++ b/premise/data/additional_inventories/lci-BIGCC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400E60F4-8CFB-1341-AF28-F7A65899BFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BE2B5A-9121-434D-8F54-8B5F31351747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35160" yWindow="1000" windowWidth="28240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1065,8 +1065,8 @@
         <v>54</v>
       </c>
       <c r="B28" s="5">
-        <f>0.49*(44/12)*B17</f>
-        <v>1.8451766666666665</v>
+        <f>1.81*B17</f>
+        <v>1.8588699999999998</v>
       </c>
       <c r="D28" t="s">
         <v>29</v>
@@ -1567,8 +1567,8 @@
         <v>54</v>
       </c>
       <c r="B58" s="5">
-        <f>0.49*(44/12)*B47*0.1</f>
-        <v>0.18451766666666666</v>
+        <f>1.81*B47*0.1</f>
+        <v>0.185887</v>
       </c>
       <c r="D58" t="s">
         <v>29</v>
@@ -1605,9 +1605,9 @@
       <c r="A60" t="s">
         <v>63</v>
       </c>
-      <c r="B60">
-        <f>0.9*1.96</f>
-        <v>1.764</v>
+      <c r="B60" s="5">
+        <f>1.81*B47*0.9</f>
+        <v>1.6729829999999999</v>
       </c>
       <c r="C60" t="s">
         <v>3</v>
@@ -2090,8 +2090,8 @@
         <v>54</v>
       </c>
       <c r="B89" s="5">
-        <f>0.49*(44/12)*B78*0.1</f>
-        <v>0.18451766666666666</v>
+        <f>1.81*B78*0.1</f>
+        <v>0.185887</v>
       </c>
       <c r="D89" t="s">
         <v>29</v>
@@ -2128,9 +2128,9 @@
       <c r="A91" t="s">
         <v>64</v>
       </c>
-      <c r="B91">
-        <f>0.9*1.96</f>
-        <v>1.764</v>
+      <c r="B91" s="5">
+        <f>1.81*B78*0.9</f>
+        <v>1.6729829999999999</v>
       </c>
       <c r="C91" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Update from master branch.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-BIGCC.xlsx
+++ b/premise/data/additional_inventories/lci-BIGCC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400E60F4-8CFB-1341-AF28-F7A65899BFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BE2B5A-9121-434D-8F54-8B5F31351747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35160" yWindow="1000" windowWidth="28240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1065,8 +1065,8 @@
         <v>54</v>
       </c>
       <c r="B28" s="5">
-        <f>0.49*(44/12)*B17</f>
-        <v>1.8451766666666665</v>
+        <f>1.81*B17</f>
+        <v>1.8588699999999998</v>
       </c>
       <c r="D28" t="s">
         <v>29</v>
@@ -1567,8 +1567,8 @@
         <v>54</v>
       </c>
       <c r="B58" s="5">
-        <f>0.49*(44/12)*B47*0.1</f>
-        <v>0.18451766666666666</v>
+        <f>1.81*B47*0.1</f>
+        <v>0.185887</v>
       </c>
       <c r="D58" t="s">
         <v>29</v>
@@ -1605,9 +1605,9 @@
       <c r="A60" t="s">
         <v>63</v>
       </c>
-      <c r="B60">
-        <f>0.9*1.96</f>
-        <v>1.764</v>
+      <c r="B60" s="5">
+        <f>1.81*B47*0.9</f>
+        <v>1.6729829999999999</v>
       </c>
       <c r="C60" t="s">
         <v>3</v>
@@ -2090,8 +2090,8 @@
         <v>54</v>
       </c>
       <c r="B89" s="5">
-        <f>0.49*(44/12)*B78*0.1</f>
-        <v>0.18451766666666666</v>
+        <f>1.81*B78*0.1</f>
+        <v>0.185887</v>
       </c>
       <c r="D89" t="s">
         <v>29</v>
@@ -2128,9 +2128,9 @@
       <c r="A91" t="s">
         <v>64</v>
       </c>
-      <c r="B91">
-        <f>0.9*1.96</f>
-        <v>1.764</v>
+      <c r="B91" s="5">
+        <f>1.81*B78*0.9</f>
+        <v>1.6729829999999999</v>
       </c>
       <c r="C91" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Add validation.py + various corrections
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-BIGCC.xlsx
+++ b/premise/data/additional_inventories/lci-BIGCC.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D010B3-D02D-5D42-9715-99BB5F4F3274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7C29E3-4FF2-ED42-857E-3EAB9C7A3DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30160" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="0.01" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="62">
   <si>
     <t>Database</t>
   </si>
@@ -206,32 +206,36 @@
     <t>inert waste</t>
   </si>
   <si>
+    <t>carbon dioxide, captured at wood burning power plant 20 MW post, pipeline 200km, storage 1000m</t>
+  </si>
+  <si>
+    <t>electricity production, at biomass-fired IGCC power plant</t>
+  </si>
+  <si>
+    <t>electricity production, at biomass-fired IGCC power plant, pre, pipeline 200km, storage 1000m</t>
+  </si>
+  <si>
     <t>The study is originally tailored to portuguese conditions, using Portugal-grown eucalyptus as biommas feedstock. The plant has a power output of 12.5 MW.
 The construciton, maintenance and operation of the plant are not from this study, but from Volkart et la, 2013. The required amounts for those have been adjusted to 12.5 MW.
-All the inventory data regarding the RFB direct gasification process were obtained from experiments carried out in a pilot-scale gasification installation running at the University of Aveiro, Portugal (Pio et al., 2017). However, data are scaled up in order to obtain the same power output of the EG-CRC power plant. At the pilot scale, the RFB is introduced in the gasification chamber by means of a screw feeder and is converted at an average temperature of 785 °C in a bubbling fluidized bed reactor of 80 kWth, operated at atmospheric pressure and under auto-thermal regime, thus, direct gasification using atmospheric air.</t>
+All the inventory data regarding the RFB direct gasification process were obtained from experiments carried out in a pilot-scale gasification installation running at the University of Aveiro, Portugal (Pio et al., 2017). However, data are scaled up in order to obtain the same power output of the EG-CRC power plant. At the pilot scale, the RFB is introduced in the gasification chamber by means of a screw feeder and is converted at an average temperature of 785 °C in a bubbling fluidized bed reactor of 80 kWth, operated at atmospheric pressure and under auto-thermal regime, thus, direct gasification using atmospheric air. Note that this study considers an electricial efficiency of 19%, which is very low compared to the rest of the literature. We scaled up this efficiency to 35%, a central estimate when considering other studies: Carpentieri et al. (2005), Puy et al. (2010), Siegl et al. (2011), Guest et al. (2011), Steubing et al. (2011), Nguyen et al. (2013), Jäppinen et al. (2014), Wang et al. (2014), Paengjuntuek et al. (2015), Cambero et al. (2015), Yang et al. (2018) and Zang et al. (2020).</t>
+  </si>
+  <si>
+    <t>Andrei Briones-Hidrovo, José Copa, Luís A.C. Tarelho, Cátia Gonçalves, Tamíris Pacheco da Costa, Ana Cláudia Dias, Environmental and energy performance of residual forest biomass for electricity generation: Gasification vs. combustion, Journal of Cleaner Production, Volume 289, 2021, 125680, ISSN 0959-6526, https://doi.org/10.1016/j.jclepro.2020.125680.</t>
   </si>
   <si>
     <t>The study is originally tailored to portuguese conditions, using Portugal-grown eucalyptus as biommas feedstock. The plant has a power output of 12.5 MW.
 Also, the original study does not include CCS. This is added from Volkart et al, 2013.
-The construciton, maintenance and operation of the plant are not from this study, but from Volkart et la, 2013. The required amounts for those have been adjusted to 12.5 MW.
-All the inventory data regarding the RFB direct gasification process were obtained from experiments carried out in a pilot-scale gasification installation running at the University of Aveiro, Portugal (Pio et al., 2017). However, data are scaled up in order to obtain the same power output of the EG-CRC power plant. At the pilot scale, the RFB is introduced in the gasification chamber by means of a screw feeder and is converted at an average temperature of 785 °C in a bubbling fluidized bed reactor of 80 kWth, operated at atmospheric pressure and under auto-thermal regime, thus, direct gasification using atmospheric air.</t>
-  </si>
-  <si>
-    <t>carbon dioxide, captured at wood burning power plant 20 MW post, pipeline 200km, storage 1000m</t>
-  </si>
-  <si>
-    <t>electricity production, at biomass-fired IGCC power plant</t>
-  </si>
-  <si>
-    <t>electricity production, at biomass-fired IGCC power plant, pre, pipeline 200km, storage 1000m</t>
+The construction, maintenance and operation of the plant are not from this study, but from Volkart et la, 2013. The required amounts for those have been adjusted to 12.5 MW.
+All the inventory data regarding the RFB direct gasification process were obtained from experiments carried out in a pilot-scale gasification installation running at the University of Aveiro, Portugal (Pio et al., 2017). However, data are scaled up in order to obtain the same power output of the EG-CRC power plant. At the pilot scale, the RFB is introduced in the gasification chamber by means of a screw feeder and is converted at an average temperature of 785 °C in a bubbling fluidized bed reactor of 80 kWth, operated at atmospheric pressure and under auto-thermal regime, thus, direct gasification using atmospheric air. Note that this study considers an electricial efficiency of 19%, which is very low compared to the rest of the literature. We scaled up this efficiency to 35%, a central estimate when considering other studies: Carpentieri et al. (2005), Puy et al. (2010), Siegl et al. (2011), Guest et al. (2011), Steubing et al. (2011), Nguyen et al. (2013), Jäppinen et al. (2014), Wang et al. (2014), Paengjuntuek et al. (2015), Cambero et al. (2015), Yang et al. (2018) and Zang et al. (2020). And then, we reduce the efficiency by approximately 10% (ie.., 30% eff.) to reflect the addendum of a CCS unit.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -278,13 +282,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,7 +572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
@@ -590,7 +595,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -637,7 +642,7 @@
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -645,8 +650,8 @@
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
-        <v>56</v>
+      <c r="B10" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -697,7 +702,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -806,8 +811,9 @@
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="B16">
-        <v>1.0269999999999999</v>
+      <c r="B16" s="6">
+        <f>(3.6/35%)/20</f>
+        <v>0.51428571428571435</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -1016,7 +1022,7 @@
       </c>
       <c r="B27" s="4">
         <f>1.81*B16</f>
-        <v>1.8588699999999998</v>
+        <v>0.93085714285714294</v>
       </c>
       <c r="D27" t="s">
         <v>29</v>
@@ -1054,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -1102,15 +1108,15 @@
         <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>19</v>
       </c>
-      <c r="B37" t="s">
-        <v>57</v>
+      <c r="B37" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -1161,7 +1167,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1270,8 +1276,9 @@
       <c r="A43" t="s">
         <v>36</v>
       </c>
-      <c r="B43">
-        <v>1.0269999999999999</v>
+      <c r="B43" s="6">
+        <f>(3.6/30%)/20</f>
+        <v>0.6</v>
       </c>
       <c r="C43" t="s">
         <v>38</v>
@@ -1480,7 +1487,7 @@
       </c>
       <c r="B54" s="4">
         <f>1.81*B43*0.1</f>
-        <v>0.185887</v>
+        <v>0.10860000000000002</v>
       </c>
       <c r="D54" t="s">
         <v>29</v>
@@ -1515,11 +1522,11 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B56" s="4">
         <f>1.81*B43*0.9</f>
-        <v>1.6729829999999999</v>
+        <v>0.97740000000000005</v>
       </c>
       <c r="C56" t="s">
         <v>3</v>
@@ -1531,7 +1538,7 @@
         <v>26</v>
       </c>
       <c r="M56" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update fuel variables for REMIND
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-BIGCC.xlsx
+++ b/premise/data/additional_inventories/lci-BIGCC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7C29E3-4FF2-ED42-857E-3EAB9C7A3DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B02993A-F2B1-A747-A49B-1BBCC5E78CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30160" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -215,18 +215,18 @@
     <t>electricity production, at biomass-fired IGCC power plant, pre, pipeline 200km, storage 1000m</t>
   </si>
   <si>
-    <t>The study is originally tailored to portuguese conditions, using Portugal-grown eucalyptus as biommas feedstock. The plant has a power output of 12.5 MW.
-The construciton, maintenance and operation of the plant are not from this study, but from Volkart et la, 2013. The required amounts for those have been adjusted to 12.5 MW.
-All the inventory data regarding the RFB direct gasification process were obtained from experiments carried out in a pilot-scale gasification installation running at the University of Aveiro, Portugal (Pio et al., 2017). However, data are scaled up in order to obtain the same power output of the EG-CRC power plant. At the pilot scale, the RFB is introduced in the gasification chamber by means of a screw feeder and is converted at an average temperature of 785 °C in a bubbling fluidized bed reactor of 80 kWth, operated at atmospheric pressure and under auto-thermal regime, thus, direct gasification using atmospheric air. Note that this study considers an electricial efficiency of 19%, which is very low compared to the rest of the literature. We scaled up this efficiency to 35%, a central estimate when considering other studies: Carpentieri et al. (2005), Puy et al. (2010), Siegl et al. (2011), Guest et al. (2011), Steubing et al. (2011), Nguyen et al. (2013), Jäppinen et al. (2014), Wang et al. (2014), Paengjuntuek et al. (2015), Cambero et al. (2015), Yang et al. (2018) and Zang et al. (2020).</t>
-  </si>
-  <si>
     <t>Andrei Briones-Hidrovo, José Copa, Luís A.C. Tarelho, Cátia Gonçalves, Tamíris Pacheco da Costa, Ana Cláudia Dias, Environmental and energy performance of residual forest biomass for electricity generation: Gasification vs. combustion, Journal of Cleaner Production, Volume 289, 2021, 125680, ISSN 0959-6526, https://doi.org/10.1016/j.jclepro.2020.125680.</t>
   </si>
   <si>
-    <t>The study is originally tailored to portuguese conditions, using Portugal-grown eucalyptus as biommas feedstock. The plant has a power output of 12.5 MW.
+    <t>The study is originally tailored to portuguese conditions, using Portugal-grown eucalyptus as biomass feedstock. The plant has a power output of 12.5 MW.
 Also, the original study does not include CCS. This is added from Volkart et al, 2013.
 The construction, maintenance and operation of the plant are not from this study, but from Volkart et la, 2013. The required amounts for those have been adjusted to 12.5 MW.
 All the inventory data regarding the RFB direct gasification process were obtained from experiments carried out in a pilot-scale gasification installation running at the University of Aveiro, Portugal (Pio et al., 2017). However, data are scaled up in order to obtain the same power output of the EG-CRC power plant. At the pilot scale, the RFB is introduced in the gasification chamber by means of a screw feeder and is converted at an average temperature of 785 °C in a bubbling fluidized bed reactor of 80 kWth, operated at atmospheric pressure and under auto-thermal regime, thus, direct gasification using atmospheric air. Note that this study considers an electricial efficiency of 19%, which is very low compared to the rest of the literature. We scaled up this efficiency to 35%, a central estimate when considering other studies: Carpentieri et al. (2005), Puy et al. (2010), Siegl et al. (2011), Guest et al. (2011), Steubing et al. (2011), Nguyen et al. (2013), Jäppinen et al. (2014), Wang et al. (2014), Paengjuntuek et al. (2015), Cambero et al. (2015), Yang et al. (2018) and Zang et al. (2020). And then, we reduce the efficiency by approximately 10% (ie.., 30% eff.) to reflect the addendum of a CCS unit.</t>
+  </si>
+  <si>
+    <t>The study is originally tailored to portuguese conditions, using Portugal-grown eucalyptus as biomass feedstock. The plant has a power output of 12.5 MW.
+The construciton, maintenance and operation of the plant are not from this study, but from Volkart et la, 2013. The required amounts for those have been adjusted to 12.5 MW.
+All the inventory data regarding the RFB direct gasification process were obtained from experiments carried out in a pilot-scale gasification installation running at the University of Aveiro, Portugal (Pio et al., 2017). However, data are scaled up in order to obtain the same power output of the EG-CRC power plant. At the pilot scale, the RFB is introduced in the gasification chamber by means of a screw feeder and is converted at an average temperature of 785 °C in a bubbling fluidized bed reactor of 80 kWth, operated at atmospheric pressure and under auto-thermal regime, thus, direct gasification using atmospheric air. Note that this study considers an electricial efficiency of 19%, which is very low compared to the rest of the literature. We scaled up this efficiency to 35%, a central estimate when considering other studies: Carpentieri et al. (2005), Puy et al. (2010), Siegl et al. (2011), Guest et al. (2011), Steubing et al. (2011), Nguyen et al. (2013), Jäppinen et al. (2014), Wang et al. (2014), Paengjuntuek et al. (2015), Cambero et al. (2015), Yang et al. (2018) and Zang et al. (2020).</t>
   </si>
 </sst>
 </file>
@@ -235,7 +235,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -288,8 +288,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -650,8 +650,8 @@
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>59</v>
+      <c r="B10" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -811,7 +811,7 @@
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <f>(3.6/35%)/20</f>
         <v>0.51428571428571435</v>
       </c>
@@ -1108,15 +1108,15 @@
         <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>61</v>
+      <c r="B37" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -1276,7 +1276,7 @@
       <c r="A43" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="5">
         <f>(3.6/30%)/20</f>
         <v>0.6</v>
       </c>

</xml_diff>